<commit_message>
File used for input to effector data
</commit_message>
<xml_diff>
--- a/effector_inputs.xlsx
+++ b/effector_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmontunnas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C1EC1-1E0F-164A-A039-5C3D25A95F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C01FBCB-F861-724C-8641-605A1943197A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{B8EEBF2D-FDDC-2849-BD58-E0F5226AEB01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Effector X (m)</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Effector Range (m)</t>
+  </si>
+  <si>
+    <t>Effector Type (0 = Fixed)</t>
   </si>
 </sst>
 </file>
@@ -416,19 +419,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885607BA-4722-BA49-B260-23ACAE5E8A31}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +442,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -449,18 +456,35 @@
       <c r="C2">
         <v>2000</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>1000</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>500</v>
       </c>
       <c r="B4">
         <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-500</v>
+      </c>
+      <c r="B6">
+        <v>-500</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created function for ensuring the nearest mobile defense is responsible for pathing towards the incoming UAS threat.
</commit_message>
<xml_diff>
--- a/effector_inputs.xlsx
+++ b/effector_inputs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmontunnas/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmontunnas/MATLAB/Projects/CAPSTONE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C01FBCB-F861-724C-8641-605A1943197A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E962D7D-7922-CA4D-A32C-5F8E27A21B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{B8EEBF2D-FDDC-2849-BD58-E0F5226AEB01}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,13 +448,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C2">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -475,16 +475,27 @@
       <c r="B4">
         <v>500</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-500</v>
       </c>
       <c r="B6">
-        <v>-500</v>
+        <v>-600</v>
       </c>
       <c r="C6">
-        <v>1000</v>
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>